<commit_message>
update role map spreadsheet
</commit_message>
<xml_diff>
--- a/docs/role.mapping.xlsx
+++ b/docs/role.mapping.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Learn.Duke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mg287/Cloud/Google Drive/dev/dukelearninginnovation/kits/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46D45C6E-EF51-474D-9914-7FC3217F1BB4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19720" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
   <si>
     <t>UI Display</t>
   </si>
   <si>
-    <t>Toolkits App Role</t>
-  </si>
-  <si>
     <t>Community Type</t>
   </si>
   <si>
@@ -44,27 +42,9 @@
     <t>Leader</t>
   </si>
   <si>
-    <t xml:space="preserve">Sakai </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WordPress </t>
-  </si>
-  <si>
     <t>CIFS</t>
   </si>
   <si>
-    <t>Wiki</t>
-  </si>
-  <si>
-    <t>Box</t>
-  </si>
-  <si>
-    <t>Sympa</t>
-  </si>
-  <si>
-    <t>Panopto</t>
-  </si>
-  <si>
     <t>Teaching Assistant</t>
   </si>
   <si>
@@ -113,12 +93,6 @@
     <t>Editor</t>
   </si>
   <si>
-    <t>Warpwire</t>
-  </si>
-  <si>
-    <t>VCL Access</t>
-  </si>
-  <si>
     <t>Non-Learning</t>
   </si>
   <si>
@@ -129,12 +103,69 @@
   </si>
   <si>
     <t>Access</t>
+  </si>
+  <si>
+    <t>Kits Role</t>
+  </si>
+  <si>
+    <t>Sakai #196</t>
+  </si>
+  <si>
+    <t>Custom URL #100</t>
+  </si>
+  <si>
+    <t>Piazza #170</t>
+  </si>
+  <si>
+    <t>Qualtrics #174</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>View/None</t>
+  </si>
+  <si>
+    <t>WordPress #212</t>
+  </si>
+  <si>
+    <t>Warpwire #213</t>
+  </si>
+  <si>
+    <t>Box #214</t>
+  </si>
+  <si>
+    <t>Sympa #215</t>
+  </si>
+  <si>
+    <t>VCM #216</t>
+  </si>
+  <si>
+    <t>Wiki #217</t>
+  </si>
+  <si>
+    <t>Panopto #218</t>
+  </si>
+  <si>
+    <t>Voicethread #219</t>
+  </si>
+  <si>
+    <t>PlayPosit #220</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,299 +485,388 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="17" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="P3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q22" t="s">
         <v>15</v>
       </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add learn.duke discovery pdf
</commit_message>
<xml_diff>
--- a/docs/role.mapping.xlsx
+++ b/docs/role.mapping.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saw38\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mg287/Cloud/Google Drive/dev/dukelearninginnovation/kits/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4A3B8688-DF75-E740-810B-5F2219878BDD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27740" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
   <si>
     <t>UI Display</t>
   </si>
@@ -203,7 +204,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -526,22 +527,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="17" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="17" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -597,7 +598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -631,6 +632,9 @@
       <c r="K2" t="s">
         <v>33</v>
       </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
       <c r="M2" t="s">
         <v>10</v>
       </c>
@@ -650,7 +654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -681,6 +685,9 @@
       <c r="K3" t="s">
         <v>21</v>
       </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
       <c r="M3" t="s">
         <v>10</v>
       </c>
@@ -700,7 +707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -731,6 +738,9 @@
       <c r="K4" t="s">
         <v>11</v>
       </c>
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
       <c r="M4" t="s">
         <v>16</v>
       </c>
@@ -750,7 +760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -781,6 +791,9 @@
       <c r="K5" t="s">
         <v>11</v>
       </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
       <c r="M5" t="s">
         <v>19</v>
       </c>
@@ -800,7 +813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -829,7 +842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>13</v>
       </c>
@@ -858,7 +871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -887,7 +900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -925,12 +938,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -947,7 +960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -964,7 +977,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -972,7 +985,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -983,7 +996,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -997,7 +1010,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -1008,7 +1021,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -1019,7 +1032,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -1030,7 +1043,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1047,7 +1060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>

</xml_diff>